<commit_message>
redaccion de breve discu y termine de hacer los resultados preliminares. Nuevo excel para hacer la tabla S6.2
</commit_message>
<xml_diff>
--- a/Data/Coexistence_Analysis/Result_Coexistence.xlsx
+++ b/Data/Coexistence_Analysis/Result_Coexistence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -3842,8 +3842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5678,8 +5678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9447,8 +9447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9617,6 +9617,10 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1094</v>
+      </c>
+      <c r="C14">
+        <f>5.84-3.38</f>
+        <v>2.46</v>
       </c>
       <c r="E14" t="s">
         <v>1107</v>
@@ -9776,8 +9780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10828,8 +10832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11445,8 +11449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>